<commit_message>
#121 - Update excel
</commit_message>
<xml_diff>
--- a/resources/docs/ReceiptTemplate.xlsx
+++ b/resources/docs/ReceiptTemplate.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\proteinpos\resources\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="540" yWindow="1200" windowWidth="11415" windowHeight="9735"/>
   </bookViews>
@@ -62,8 +57,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,14 +223,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -282,7 +269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -314,27 +301,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -366,24 +335,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -559,17 +510,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="15" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" style="15" customWidth="1"/>
@@ -577,37 +528,37 @@
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -615,7 +566,7 @@
       <c r="C6" s="18"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -623,7 +574,7 @@
       <c r="C7" s="11"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="20" t="s">
         <v>2</v>
       </c>
@@ -631,7 +582,7 @@
       <c r="C8" s="16"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="23" t="s">
         <v>9</v>
       </c>
@@ -639,7 +590,7 @@
       <c r="C9" s="18"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="23" t="s">
         <v>10</v>
       </c>
@@ -647,7 +598,7 @@
       <c r="C10" s="11"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="25" t="s">
         <v>11</v>
       </c>
@@ -655,7 +606,7 @@
       <c r="C11" s="16"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
@@ -667,61 +618,61 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="2.25" customHeight="1">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="7"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="21"/>
       <c r="B14" s="22"/>
       <c r="C14" s="21"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="9"/>
       <c r="B15" s="10"/>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="12"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="9"/>
       <c r="B18" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="17"/>
       <c r="B19" s="16"/>
       <c r="C19" s="17"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="9"/>
       <c r="B20" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="14"/>
       <c r="B21" s="4"/>
       <c r="C21" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.2" right="0.1" top="0.5" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="32767" fitToWidth="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="32767" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;C
 &amp;G
@@ -738,26 +689,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>